<commit_message>
Updating skills TODO.xlsx file.
</commit_message>
<xml_diff>
--- a/dist/game/data/stats/skills/TODO.xlsx
+++ b/dist/game/data/stats/skills/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="556">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2079,7 +2079,7 @@
   <dimension ref="A1:G590"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="G2" s="5">
         <f>COUNTIF(C2:C590,"yes")</f>
-        <v>408</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="G3">
         <f>589-G2</f>
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2163,7 +2163,7 @@
       </c>
       <c r="G4" s="7">
         <f>100-(G3*100)/589</f>
-        <v>69.269949066213925</v>
+        <v>70.288624787775888</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6807,7 +6807,9 @@
       <c r="B410" s="2">
         <v>11538</v>
       </c>
-      <c r="C410" s="3"/>
+      <c r="C410" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D410" s="2"/>
     </row>
     <row r="411" spans="1:4">
@@ -6817,7 +6819,9 @@
       <c r="B411" s="2">
         <v>11539</v>
       </c>
-      <c r="C411" s="3"/>
+      <c r="C411" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D411" s="2"/>
     </row>
     <row r="412" spans="1:4">
@@ -6993,7 +6997,9 @@
       <c r="B426" s="2">
         <v>11557</v>
       </c>
-      <c r="C426" s="3"/>
+      <c r="C426" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D426" s="2"/>
     </row>
     <row r="427" spans="1:4">
@@ -7003,7 +7009,9 @@
       <c r="B427" s="2">
         <v>11558</v>
       </c>
-      <c r="C427" s="3"/>
+      <c r="C427" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D427" s="2"/>
     </row>
     <row r="428" spans="1:4">
@@ -7013,7 +7021,9 @@
       <c r="B428" s="2">
         <v>11559</v>
       </c>
-      <c r="C428" s="3"/>
+      <c r="C428" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D428" s="2"/>
     </row>
     <row r="429" spans="1:4">
@@ -7035,7 +7045,9 @@
       <c r="B430" s="2">
         <v>11561</v>
       </c>
-      <c r="C430" s="3"/>
+      <c r="C430" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D430" s="2"/>
     </row>
     <row r="431" spans="1:4">

</xml_diff>

<commit_message>
Updated skills TODO file.
</commit_message>
<xml_diff>
--- a/dist/game/data/stats/skills/TODO.xlsx
+++ b/dist/game/data/stats/skills/TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11955"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12990" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="SkillList" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="556">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2079,7 +2079,7 @@
   <dimension ref="A1:G590"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="G2" s="5">
         <f>COUNTIF(C2:C590,"yes")</f>
-        <v>414</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="G3">
         <f>589-G2</f>
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2163,7 +2163,7 @@
       </c>
       <c r="G4" s="7">
         <f>100-(G3*100)/589</f>
-        <v>70.288624787775888</v>
+        <v>71.307300509337864</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3239,7 +3239,9 @@
       <c r="B95" s="2">
         <v>10073</v>
       </c>
-      <c r="C95" s="3"/>
+      <c r="C95" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D95" s="2"/>
     </row>
     <row r="96" spans="1:4">
@@ -3273,7 +3275,7 @@
       <c r="B98" s="2">
         <v>10077</v>
       </c>
-      <c r="C98" s="3"/>
+      <c r="C98" s="2"/>
       <c r="D98" s="2"/>
     </row>
     <row r="99" spans="1:4">
@@ -3283,7 +3285,9 @@
       <c r="B99" s="2">
         <v>10079</v>
       </c>
-      <c r="C99" s="3"/>
+      <c r="C99" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="1:4">
@@ -3293,7 +3297,9 @@
       <c r="B100" s="2">
         <v>10080</v>
       </c>
-      <c r="C100" s="3"/>
+      <c r="C100" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D100" s="2"/>
     </row>
     <row r="101" spans="1:4">
@@ -3313,7 +3319,9 @@
       <c r="B102" s="2">
         <v>10092</v>
       </c>
-      <c r="C102" s="3"/>
+      <c r="C102" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D102" s="2"/>
     </row>
     <row r="103" spans="1:4">
@@ -5975,7 +5983,9 @@
       <c r="B336" s="2">
         <v>11268</v>
       </c>
-      <c r="C336" s="3"/>
+      <c r="C336" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D336" s="2"/>
     </row>
     <row r="337" spans="1:4">
@@ -7545,7 +7555,9 @@
       <c r="B474" s="2">
         <v>11754</v>
       </c>
-      <c r="C474" s="3"/>
+      <c r="C474" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D474" s="2"/>
     </row>
     <row r="475" spans="1:4">

</xml_diff>

<commit_message>
-TriggerForce effect for awaken class forces. -Forces (except Eviscerator - temp done, need correct stat). -Update TriggerForce effect and implemented all Sigel's Aura buffs/debuff.
Contributed by NviX.
</commit_message>
<xml_diff>
--- a/dist/game/data/stats/skills/TODO.xlsx
+++ b/dist/game/data/stats/skills/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="556">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="G2" s="5">
         <f>COUNTIF(C2:C590,"yes")</f>
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="G3">
         <f>589-G2</f>
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2163,7 +2163,7 @@
       </c>
       <c r="G4" s="7">
         <f>100-(G3*100)/589</f>
-        <v>71.307300509337864</v>
+        <v>72.835314091680814</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2569,7 +2569,9 @@
       <c r="B38" s="2">
         <v>1927</v>
       </c>
-      <c r="C38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4">
@@ -2579,7 +2581,9 @@
       <c r="B39" s="2">
         <v>1929</v>
       </c>
-      <c r="C39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4">
@@ -2589,7 +2593,9 @@
       <c r="B40" s="2">
         <v>1931</v>
       </c>
-      <c r="C40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4">
@@ -2599,7 +2605,9 @@
       <c r="B41" s="2">
         <v>1933</v>
       </c>
-      <c r="C41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4">
@@ -2609,7 +2617,9 @@
       <c r="B42" s="2">
         <v>1935</v>
       </c>
-      <c r="C42" s="3"/>
+      <c r="C42" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4">
@@ -2619,7 +2629,9 @@
       <c r="B43" s="2">
         <v>1937</v>
       </c>
-      <c r="C43" s="3"/>
+      <c r="C43" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4">
@@ -2629,7 +2641,9 @@
       <c r="B44" s="2">
         <v>1939</v>
       </c>
-      <c r="C44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4">
@@ -8847,7 +8861,9 @@
       <c r="B589" s="2">
         <v>30602</v>
       </c>
-      <c r="C589" s="3"/>
+      <c r="C589" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D589" s="2"/>
     </row>
     <row r="590" spans="1:4">
@@ -8857,7 +8873,9 @@
       <c r="B590" s="2">
         <v>30605</v>
       </c>
-      <c r="C590" s="3"/>
+      <c r="C590" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D590" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Craft Mastery skill (10312).
</commit_message>
<xml_diff>
--- a/dist/game/data/stats/skills/TODO.xlsx
+++ b/dist/game/data/stats/skills/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="556">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2078,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G590"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="G2" s="5">
         <f>COUNTIF(C2:C590,"yes")</f>
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="G3">
         <f>589-G2</f>
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2163,7 +2163,7 @@
       </c>
       <c r="G4" s="7">
         <f>100-(G3*100)/589</f>
-        <v>85.568760611205434</v>
+        <v>85.73853989813243</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3983,7 +3983,9 @@
       <c r="B156" s="2">
         <v>10312</v>
       </c>
-      <c r="C156" s="3"/>
+      <c r="C156" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D156" s="2"/>
     </row>
     <row r="157" spans="1:4">

</xml_diff>

<commit_message>
Skills Diversion (10778), Remote Control (10788) and Superior Skill Mastery (10904). Contributed by Sahar.
</commit_message>
<xml_diff>
--- a/dist/game/data/stats/skills/TODO.xlsx
+++ b/dist/game/data/stats/skills/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="556">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2078,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="G2" s="5">
         <f>COUNTIF(C2:C590,"yes")</f>
-        <v>505</v>
+        <v>509</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="G3">
         <f>589-G2</f>
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2163,7 +2163,7 @@
       </c>
       <c r="G4" s="7">
         <f>100-(G3*100)/589</f>
-        <v>85.73853989813243</v>
+        <v>86.4176570458404</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3913,7 +3913,9 @@
       <c r="B150" s="2">
         <v>10301</v>
       </c>
-      <c r="C150" s="3"/>
+      <c r="C150" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D150" s="2"/>
     </row>
     <row r="151" spans="1:4">
@@ -4991,7 +4993,9 @@
       <c r="B240" s="2">
         <v>10778</v>
       </c>
-      <c r="C240" s="3"/>
+      <c r="C240" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D240" s="2"/>
     </row>
     <row r="241" spans="1:4">
@@ -5097,7 +5101,9 @@
       <c r="B249" s="2">
         <v>10788</v>
       </c>
-      <c r="C249" s="3"/>
+      <c r="C249" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D249" s="2"/>
     </row>
     <row r="250" spans="1:4">
@@ -5263,7 +5269,9 @@
       <c r="B263" s="2">
         <v>10904</v>
       </c>
-      <c r="C263" s="3"/>
+      <c r="C263" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D263" s="2"/>
     </row>
     <row r="264" spans="1:4">

</xml_diff>

<commit_message>
Updated skills 11853, 11151, 11176, 11183, 11184, 11255, 11540 and 11550.
</commit_message>
<xml_diff>
--- a/dist/game/data/stats/skills/TODO.xlsx
+++ b/dist/game/data/stats/skills/TODO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="556">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="G2" s="5">
         <f>COUNTIF(C2:C590,"yes")</f>
-        <v>509</v>
+        <v>515</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="G3">
         <f>589-G2</f>
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2163,7 +2163,7 @@
       </c>
       <c r="G4" s="7">
         <f>100-(G3*100)/589</f>
-        <v>86.4176570458404</v>
+        <v>87.436332767402376</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5797,7 +5797,9 @@
       <c r="B308" s="2">
         <v>11151</v>
       </c>
-      <c r="C308" s="3"/>
+      <c r="C308" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D308" s="2"/>
     </row>
     <row r="309" spans="1:4">
@@ -5817,7 +5819,9 @@
       <c r="B310" s="2">
         <v>11176</v>
       </c>
-      <c r="C310" s="3"/>
+      <c r="C310" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D310" s="2"/>
     </row>
     <row r="311" spans="1:4">
@@ -5837,7 +5841,9 @@
       <c r="B312" s="2">
         <v>11183</v>
       </c>
-      <c r="C312" s="3"/>
+      <c r="C312" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D312" s="2"/>
     </row>
     <row r="313" spans="1:4">
@@ -5967,7 +5973,9 @@
       <c r="B323" s="2">
         <v>11255</v>
       </c>
-      <c r="C323" s="3"/>
+      <c r="C323" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D323" s="2"/>
     </row>
     <row r="324" spans="1:4">
@@ -7075,7 +7083,9 @@
       <c r="B420" s="2">
         <v>11549</v>
       </c>
-      <c r="C420" s="3"/>
+      <c r="C420" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D420" s="2"/>
     </row>
     <row r="421" spans="1:4">
@@ -8299,7 +8309,9 @@
       <c r="B525" s="2">
         <v>11853</v>
       </c>
-      <c r="C525" s="3"/>
+      <c r="C525" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="D525" s="2"/>
     </row>
     <row r="526" spans="1:4">

</xml_diff>